<commit_message>
Update node Nội trú > Điều trị nội trú > In ký số > Giấy hẹn khám via tool
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -451,10 +451,10 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>44444</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_k_s_Giy_hn_khm_1762098234476_0.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_k_s_Giy_hn_khm_1762098235932_1.webp</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Update node Nội trú > Điều trị nội trú > In ký số > Phiếu công khai dịch vụ via tool
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -477,10 +477,10 @@
         <v/>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>33333</v>
       </c>
       <c r="H3" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_k_s_Phiu_cng_khai_dch_v_1762098334306_0.webp</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Update node Nội trú > Điều trị nội trú > In ấn > Giấy hẹn khám doc via tool
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -1519,10 +1519,10 @@
         <v/>
       </c>
       <c r="G43" t="str">
-        <v/>
+        <v>6666666666666</v>
       </c>
       <c r="H43" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098707463_0.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098708977_1.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098711189_2.webp</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Điều trị nội trú > In ký số > Giấy hẹn khám
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -451,10 +451,10 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <v>44444</v>
+        <v>66666666666</v>
       </c>
       <c r="H2" t="str">
-        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_k_s_Giy_hn_khm_1762098234476_0.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_k_s_Giy_hn_khm_1762098235932_1.webp</v>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762099834218_pasted_1762099828065.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762099835780_pasted_1762099830029.webp</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Hành chính nội trú > In ký số > Giấy hẹn khám lại
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -5029,10 +5029,10 @@
         <v/>
       </c>
       <c r="G178" t="str">
-        <v/>
+        <v>666666666</v>
       </c>
       <c r="H178" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762099909720_pasted_1762099907496.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762099911074_pasted_1762099908582.webp</v>
       </c>
     </row>
     <row r="179">

</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Điều trị nội trú > In ấn > Giấy hẹn khám doc
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -1519,10 +1519,10 @@
         <v/>
       </c>
       <c r="G43" t="str">
-        <v>6666666666666</v>
+        <v/>
       </c>
       <c r="H43" t="str">
-        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098707463_0.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098708977_1.webp; https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Ni_tr_iu_tr_ni_tr_In_n_Giy_hn_khm_doc_1762098711189_2.webp</v>
+        <v/>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Điều trị nội trú > In ấn > Đơn thuốc
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -633,10 +633,10 @@
         <v/>
       </c>
       <c r="G9" t="str">
-        <v/>
+        <v>11111</v>
       </c>
       <c r="H9" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762102389634_Screenshot_3.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762102391059_Screenshot_2.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762102392294_pasted_1762102388220.webp</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Thêm node mới: HDSD > Hướng dẫn sử dụng
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1143"/>
+  <dimension ref="A1:H1144"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30251,9 +30251,35 @@
         <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Screenshot_1762017495834.webp</v>
       </c>
     </row>
+    <row r="1144">
+      <c r="A1144" t="str">
+        <v>Hướng dẫn sử dụng</v>
+      </c>
+      <c r="B1144" t="str">
+        <v/>
+      </c>
+      <c r="C1144" t="str">
+        <v/>
+      </c>
+      <c r="D1144" t="str">
+        <v/>
+      </c>
+      <c r="E1144" t="str">
+        <v/>
+      </c>
+      <c r="F1144" t="str">
+        <v/>
+      </c>
+      <c r="G1144" t="str">
+        <v/>
+      </c>
+      <c r="H1144" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1143"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1144"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Thêm node mới: Hướng dẫn sử dụng > Hướng dẫn sử dụng liên thông HIS - LIS
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1144"/>
+  <dimension ref="A1:H1145"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30277,9 +30277,50 @@
         <v/>
       </c>
     </row>
+    <row r="1145" xml:space="preserve">
+      <c r="A1145" t="str">
+        <v>Hướng dẫn sử dụng liên thông HIS - LIS</v>
+      </c>
+      <c r="B1145" t="str">
+        <v/>
+      </c>
+      <c r="C1145" t="str">
+        <v/>
+      </c>
+      <c r="D1145" t="str">
+        <v/>
+      </c>
+      <c r="E1145" t="str">
+        <v/>
+      </c>
+      <c r="F1145" t="str">
+        <v/>
+      </c>
+      <c r="G1145" t="str" xml:space="preserve">
+        <v xml:space="preserve">Bước 1: Tạo Tài khoản tích hợp trên his:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC13_QL_NguoiDung  
+  + cấu hình "Mức truy cập": Nghiệp vụ  
+  + Loại tài khoản: Tích hợp  
+Bước 2: Phần quyền dữ liệu người dùng:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC10_user_role  
+  + Theo quyền dữ liệu được cấu hình theo khoa phòng thực hiện  
+Bước 3: Cấu hình tham số:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC02_CAUHINHLIS_UPDATE_STATUS
+LIS_DELETE_REQUEST  api/v2/DeleteRequest  Địa chỉ service để xóa chỉ định khỏi hệ thống LIS              
+LIS_SEND_REQUEST  api/v2/SendRequest  Địa chỉ service để gửi chỉ định sang hệ thống LIS              
+LIS_GET_RESULT_SET  api/v2/GetResultSet  Địa chỉ service lấy kết quả từ hệ thống LIS              
+LIS_SERVICE_DOMAIN_NAME  https://lisdkhnm.vnptsoftware.vn/  Tên địa chỉ domain service LIS              
+LIS_SECRET_KEY  123456  Mật khẩu truy cập hệ thống VNPT LIS              
+LIS_CONNECTION_TYPE = 1
+LIS_DIACHI_BENHNHAN = bhyt hoặc bn</v>
+      </c>
+      <c r="H1145" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1144"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Thêm node mới: Hướng dẫn sử dụng > HDSD
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1145"/>
+  <dimension ref="A1:H1146"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30318,9 +30318,35 @@
         <v/>
       </c>
     </row>
+    <row r="1146">
+      <c r="A1146" t="str">
+        <v>HDSD</v>
+      </c>
+      <c r="B1146" t="str">
+        <v/>
+      </c>
+      <c r="C1146" t="str">
+        <v/>
+      </c>
+      <c r="D1146" t="str">
+        <v/>
+      </c>
+      <c r="E1146" t="str">
+        <v/>
+      </c>
+      <c r="F1146" t="str">
+        <v/>
+      </c>
+      <c r="G1146" t="str">
+        <v>222222</v>
+      </c>
+      <c r="H1146" t="str">
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123770823_pasted_1762123765387.webp</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1146"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật node Hướng dẫn sử dụng > Hướng dẫn sử dụng
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -30271,10 +30271,10 @@
         <v/>
       </c>
       <c r="G1144" t="str">
-        <v/>
+        <v>222222222222</v>
       </c>
       <c r="H1144" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123913395_pasted_1762123908749.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123914854_pasted_1762123912180.webp</v>
       </c>
     </row>
     <row r="1145" xml:space="preserve">

</xml_diff>

<commit_message>
Cập nhật node HDSD > HDSD
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -30338,10 +30338,10 @@
         <v/>
       </c>
       <c r="G1146" t="str">
-        <v>222222</v>
+        <v/>
       </c>
       <c r="H1146" t="str">
-        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123770823_pasted_1762123765387.webp</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xóa node: HDSD > HDSD
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1146"/>
+  <dimension ref="A1:H1145"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30318,35 +30318,9 @@
         <v/>
       </c>
     </row>
-    <row r="1146">
-      <c r="A1146" t="str">
-        <v>HDSD</v>
-      </c>
-      <c r="B1146" t="str">
-        <v/>
-      </c>
-      <c r="C1146" t="str">
-        <v/>
-      </c>
-      <c r="D1146" t="str">
-        <v/>
-      </c>
-      <c r="E1146" t="str">
-        <v/>
-      </c>
-      <c r="F1146" t="str">
-        <v/>
-      </c>
-      <c r="G1146" t="str">
-        <v/>
-      </c>
-      <c r="H1146" t="str">
-        <v/>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1146"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Hành chính nội trú > Chọn BN --> Chuột phải > Thêm phiếu > Phiếu theo dõi và chăm sóc cấp 1 (BVTL)
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -9189,10 +9189,10 @@
         <v/>
       </c>
       <c r="G338" t="str">
-        <v/>
+        <v>111111111111</v>
       </c>
       <c r="H338" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762131116332_pasted_1762131109538.webp</v>
       </c>
     </row>
     <row r="339">

</xml_diff>

<commit_message>
Cập nhật node Nội trú  > Nội trú  > Hành chính nội trú > Điều trị > Tạo phiếu chăm sóc cấp II, III
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -7245,7 +7245,7 @@
         <v/>
       </c>
     </row>
-    <row r="264">
+    <row r="264" xml:space="preserve">
       <c r="A264" t="str">
         <v xml:space="preserve">Nội trú </v>
       </c>
@@ -7264,11 +7264,40 @@
       <c r="F264" t="str">
         <v/>
       </c>
-      <c r="G264" t="str">
-        <v/>
+      <c r="G264" t="str" xml:space="preserve">
+        <v xml:space="preserve">Hướng dẫn sử dụng phiếu theo dõi và chăm sóc
+Thông tin người bệnh:
+1. Ghi chính xác và thống nhất giữa các phiếu trong Hồ sơ.
+Nhận định, theo dõi:
+1. Chỉ số sinh tồn, sinh trắc: ghi giá trị bằng số.
+2. Toàn thân, hô hấp, tuần hoàn, dinh dưỡng, giấc ngủ, nghỉ ngơi, vệ sinh cá nhân, tinh thần, vận động, PHCN, GDSK: ghi rõ nội dung nhận định hoặc xây dựng các nội dung nhận định và mã hóa.
+VD: Da, niêm mạc có thể ghi rõ nội dung hoặc mã hóa là: 01. Hồng; 02. Vàng; 03 Nhợt nhạt
+Chú ý: để tạo thuận lợi cho việc nhận định và tùy thuộc nội dung nhận định, việc xây dựng nên có 1 mã “Bình thường” và các mã bệnh lý. 
+3. Một số thang đo gợi ý áp dụng bao gồm:
+	Đau (Với trẻ sơ sinh sử dụng thang điểm như NIPS (Neonatal Infant Pain Scale - Thang đo mức độ đau của trẻ sơ sinh); với trẻ dưới 7 tuổi sử dụng thang điểm như FLACC ((Face, Legs, Actitivity, Cry, Consolability - Mặt, chân, hoạt động, khóc, Đáp ứng khi được dỗ dành); với trẻ trên 7 tuổi sử dụng thang điểm như VAS (Visual Analog Scale – Thang đo trực quan tương ứng).
+	Phù: Mức độ phù sử dụng thang điểm đánh giá như phân loại từ 1 - 4 (Độ 1: ấn lõm &lt; 2 mm, biến mất ngay lập tức; Độ 2: ấn lõm 2 - 4 mm, biến mất sau 10 – 15 giây; Độ 3: ấn lõm 4 - 6 mm, có thể tồn tại  &gt; 1 phút; Độ 4: ấn lõm 6 - 8 mm, có thể tồn tại từ 2 – 5 phút).
+	Nguy cơ té ngã (sử dụng thang điểm như Morse).
+	Nguy cơ loét do tỳ đè (sử dụng thang điểm đánh giá như Braden).
+	Cảnh báo sớm (sử dụng bảng điểm cảnh báo sớm như NEWS2).
+	Đánh giá mức độ viêm tĩnh mạch (sử dụng thang điểm như VIP Score).
+Can thiệp điều dưỡng:
+Ghi rõ nội dung can thiệp hoặc xây dựng các nội dung can thiệp và mã hóa (Cột ngoài cùng bên phải hoặc trên trang khác tùy theo số lượng mã hóa).
+VD: Ký hiệu theo phân theo các nhóm như Hô hấp có các mã H01. Hướng dẫn ho khạc đờm, vỗ lưng, giữ ấm cổ ngực; H02 - Cung cấp Oxy...; Tuần hoàn có các mã T01- Nằm đầu thấp, T02 - Hạn chế vận động...
+Hoặc ký hiệu theo thứ tự quy ước như 01 - Theo dõi DHST, 02- Thở oxy, 03- Vỗ rung, uống nước ấm…
+Bàn giao
+Xây dựng các nội dung bàn giao theo đặc thù chung của cơ sở khám bệnh, chữa bệnh.
+VD: Bàn giao hồ sơ, phim, người bệnh,…
+Chẩn đoán điều dưỡng/Đánh giá mục tiêu:
+1. Xây dựng chẩn đoán điều dưỡng và đưa ra các mục tiêu chăm sóc đối với từng chẩn đoán. Chẩn đoán điều dưỡng được xây dựng khi người bệnh nhập khoa và sẽ cập nhật khi người bệnh có phát sinh những vấn đề hoặc nhu cầu mới.
+2. Thực hiện đánh giá/lượng giá mục tiêu chăm sóc: đánh dấu (X) vào các ô mục tiêu sau khi đã hoàn thành.
+Ví dụ: Chẩn đoán ĐD “người bệnh khó chịu do vệ sinh cá nhân kém”.
+⬜ Mục tiêu “người bệnh vệ sinh cá nhân sạch sẽ”: chưa hoàn thành.
+❎ Mục tiêu “người bệnh vệ sinh cá nhân sạch sẽ”: hoàn thành.
+3. Mục tiêu chưa hoàn thành (Không đánh dấu (X)): sẽ tiếp tục thực hiện hoặc thay đổi mục tiêu theo vấn đề hiện tại của người bệnh. 
+4. Trường hợp khi người bệnh xuất viện nhưng các mục tiêu chăm sóc chưa hoàn thành, điều dưỡng tiến hành tư vấn và hướng dẫn người bệnh tiếp tục chăm sóc tại nhà.</v>
       </c>
       <c r="H264" t="str">
-        <v/>
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762133076151_pasted_1762133051528.webp</v>
       </c>
     </row>
     <row r="265">

</xml_diff>

<commit_message>
Thêm node mới: Hướng dẫn sử dụng > Hướng dẫn liên thông HIS - LIS
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1145"/>
+  <dimension ref="A1:H1146"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30347,9 +30347,51 @@
         <v/>
       </c>
     </row>
+    <row r="1146" xml:space="preserve">
+      <c r="A1146" t="str">
+        <v>Hướng dẫn liên thông HIS - LIS</v>
+      </c>
+      <c r="B1146" t="str">
+        <v/>
+      </c>
+      <c r="C1146" t="str">
+        <v/>
+      </c>
+      <c r="D1146" t="str">
+        <v/>
+      </c>
+      <c r="E1146" t="str">
+        <v/>
+      </c>
+      <c r="F1146" t="str">
+        <v/>
+      </c>
+      <c r="G1146" t="str" xml:space="preserve">
+        <v xml:space="preserve">Bước 1: Tạo Tài khoản tích hợp trên his:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC13_QL_NguoiDung  
+  + cấu hình "Mức truy cập": Nghiệp vụ  
+  + Loại tài khoản: Tích hợp  
+Bước 2: Phần quyền dữ liệu người dùng:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC10_user_role  
+  + Theo quyền dữ liệu được cấu hình theo khoa phòng thực hiện  
+Bước 3: Cấu hình tham số:    
+  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC02_CAUHINHLIS_UPDATE_STATUS
+LIS_DELETE_REQUEST  api/v2/DeleteRequest  Địa chỉ service để xóa chỉ định khỏi hệ thống LIS              
+LIS_SEND_REQUEST  api/v2/SendRequest  Địa chỉ service để gửi chỉ định sang hệ thống LIS              
+LIS_GET_RESULT_SET  api/v2/GetResultSet  Địa chỉ service lấy kết quả từ hệ thống LIS              
+LIS_SERVICE_DOMAIN_NAME  https://lisdkhnm.vnptsoftware.vn/  Tên địa chỉ domain service LIS              
+LIS_SECRET_KEY  123456  Mật khẩu truy cập hệ thống VNPT LIS              
+LIS_CONNECTION_TYPE = 1
+LIS_DIACHI_BENHNHAN = bhyt hoặc bn
+</v>
+      </c>
+      <c r="H1146" t="str">
+        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762134705868_pasted_1762134704400.webp</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1146"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Xóa toàn bộ dòng: Hướng dẫn liên thông HIS - LIS
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1146"/>
+  <dimension ref="A1:H1145"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30347,51 +30347,9 @@
         <v/>
       </c>
     </row>
-    <row r="1146" xml:space="preserve">
-      <c r="A1146" t="str">
-        <v>Hướng dẫn liên thông HIS - LIS</v>
-      </c>
-      <c r="B1146" t="str">
-        <v/>
-      </c>
-      <c r="C1146" t="str">
-        <v/>
-      </c>
-      <c r="D1146" t="str">
-        <v/>
-      </c>
-      <c r="E1146" t="str">
-        <v/>
-      </c>
-      <c r="F1146" t="str">
-        <v/>
-      </c>
-      <c r="G1146" t="str" xml:space="preserve">
-        <v xml:space="preserve">Bước 1: Tạo Tài khoản tích hợp trên his:    
-  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC13_QL_NguoiDung  
-  + cấu hình "Mức truy cập": Nghiệp vụ  
-  + Loại tài khoản: Tích hợp  
-Bước 2: Phần quyền dữ liệu người dùng:    
-  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC10_user_role  
-  + Theo quyền dữ liệu được cấu hình theo khoa phòng thực hiện  
-Bước 3: Cấu hình tham số:    
-  + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC02_CAUHINHLIS_UPDATE_STATUS
-LIS_DELETE_REQUEST  api/v2/DeleteRequest  Địa chỉ service để xóa chỉ định khỏi hệ thống LIS              
-LIS_SEND_REQUEST  api/v2/SendRequest  Địa chỉ service để gửi chỉ định sang hệ thống LIS              
-LIS_GET_RESULT_SET  api/v2/GetResultSet  Địa chỉ service lấy kết quả từ hệ thống LIS              
-LIS_SERVICE_DOMAIN_NAME  https://lisdkhnm.vnptsoftware.vn/  Tên địa chỉ domain service LIS              
-LIS_SECRET_KEY  123456  Mật khẩu truy cập hệ thống VNPT LIS              
-LIS_CONNECTION_TYPE = 1
-LIS_DIACHI_BENHNHAN = bhyt hoặc bn
-</v>
-      </c>
-      <c r="H1146" t="str">
-        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762134705868_pasted_1762134704400.webp</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1146"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Xóa node: Hướng dẫn sử dụng > Hướng dẫn sử dụng
</commit_message>
<xml_diff>
--- a/data_hisl2.xlsx
+++ b/data_hisl2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1145"/>
+  <dimension ref="A1:H1144"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -30280,9 +30280,9 @@
         <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/Screenshot_1762017495834.webp</v>
       </c>
     </row>
-    <row r="1144">
+    <row r="1144" xml:space="preserve">
       <c r="A1144" t="str">
-        <v>Hướng dẫn sử dụng</v>
+        <v>Hướng dẫn sử dụng liên thông HIS - LIS</v>
       </c>
       <c r="B1144" t="str">
         <v/>
@@ -30299,33 +30299,7 @@
       <c r="F1144" t="str">
         <v/>
       </c>
-      <c r="G1144" t="str">
-        <v>222222222222</v>
-      </c>
-      <c r="H1144" t="str">
-        <v>https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123913395_pasted_1762123908749.webp;https://raw.githack.com/huongnxhni/image_hisl2/main/thumbs/1762123914854_pasted_1762123912180.webp</v>
-      </c>
-    </row>
-    <row r="1145" xml:space="preserve">
-      <c r="A1145" t="str">
-        <v>Hướng dẫn sử dụng liên thông HIS - LIS</v>
-      </c>
-      <c r="B1145" t="str">
-        <v/>
-      </c>
-      <c r="C1145" t="str">
-        <v/>
-      </c>
-      <c r="D1145" t="str">
-        <v/>
-      </c>
-      <c r="E1145" t="str">
-        <v/>
-      </c>
-      <c r="F1145" t="str">
-        <v/>
-      </c>
-      <c r="G1145" t="str" xml:space="preserve">
+      <c r="G1144" t="str" xml:space="preserve">
         <v xml:space="preserve">Bước 1: Tạo Tài khoản tích hợp trên his:    
   + Link chức năng: /vnpthis/main/manager.jsp?func=../danhmuc/DMC13_QL_NguoiDung  
   + cấu hình "Mức truy cập": Nghiệp vụ  
@@ -30343,13 +30317,13 @@
 LIS_CONNECTION_TYPE = 1
 LIS_DIACHI_BENHNHAN = bhyt hoặc bn</v>
       </c>
-      <c r="H1145" t="str">
+      <c r="H1144" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1145"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1144"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>